<commit_message>
fix list add function
</commit_message>
<xml_diff>
--- a/insertDB/steadyRank.xlsx
+++ b/insertDB/steadyRank.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1098,6 +1098,266 @@
       </c>
       <c r="C51" t="n">
         <v>31450</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>484</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">배당 </t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>31399</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>1509</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>행사 가격</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>30943</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>327</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>환율</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>30930</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>1051</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>그린채권</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>30483</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>1744</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>중화</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>29320</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>586</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>유럽연합</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>29071</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>1013</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>결산</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>28483</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>시가총액</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>28475</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>1104</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>디지털 금융</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>28419</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>1698</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>입찰</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>27618</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>1450</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>부가가치</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>27587</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>541</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>시공사</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>26038</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>686</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>추가경정예산</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>25981</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>423</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>국세</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>25943</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>2025</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>독점</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>25828</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>613</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>재건축</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>25610</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>833</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>소셜네트워크서비스</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>25303</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>작은 정부</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>24791</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>944</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>당기순이익</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>24115</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>1704</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>자기자본</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>23921</v>
       </c>
     </row>
   </sheetData>
@@ -1111,7 +1371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1779,6 +2039,266 @@
       </c>
       <c r="C51" t="n">
         <v>4378</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>재개발</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>4363</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>320</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>부담금</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4358</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>범위의 경제</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>4358</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>769</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>빅뱅</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4346</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>1030</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>수재</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>4308</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>518</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>디지털 경제</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>4304</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>1038</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>CBS</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4285</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>인구 고령화</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4258</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>695</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>금융감독원</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>1274</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>기본 소득</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>1306</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>독점</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>404</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>저작권</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>4068</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>593</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>트위터</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>965</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>홀딩스</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>3947</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>1245</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>공정거래위원회</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>3916</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>781</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>상환</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>1207</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>PER</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>3851</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>1040</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>EaR</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">직접 금융 </t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>3724</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>535</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>CEO</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3718</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +2312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2460,6 +2980,266 @@
       </c>
       <c r="C51" t="n">
         <v>16311</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>1383</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>홀딩스</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>16305</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>1796</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>기준금리</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>15725</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>1320</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>부가가치</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>15518</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>1038</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>보합세</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>14826</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>1193</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>유가증권</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>14793</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>750</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>스마트 자동차</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>14761</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>613</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>출연</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>14596</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>1072</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>상품권</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>14536</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>1743</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>고용없는 성장</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>14502</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>1459</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>CTO</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>14276</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>302</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>구조조정</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>14240</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>1546</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>자본 경영</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>13955</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>1772</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>국내총생산</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>13954</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>822</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>13853</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>1730</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>경제성장률</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>13764</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>1220</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>임대료</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>13669</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>제품 차별화</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>13200</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>1631</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>판매 채널</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>13167</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>526</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>유럽연합</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>13106</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>1352</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>핀테크</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>12881</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +3253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3141,6 +3921,266 @@
       </c>
       <c r="C51" t="n">
         <v>2329</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>재개발</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>2311</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>부의 효과</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>2257</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>648</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>빅뱅</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>535</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LaR</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>459</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>스마트 교육</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>487</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>증강현실</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>486</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>점포자동화</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>663</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>소득 대비 대출 비율</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>605</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>넉아웃</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>447</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>빅데이터</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>그린슈트</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>274</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">배당 </t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>1098</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>규모의 경제</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>899</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>엑시트</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>580</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>COO</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>842</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>밀레니얼 세대</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>1003</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>779</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>콜</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>연금</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>환경 경영</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>1520</v>
       </c>
     </row>
   </sheetData>
@@ -3154,7 +4194,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3824,6 +4864,266 @@
         <v>5336</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>1311</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>규모의 경제</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>5109</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>700</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>금융감독원</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>5053</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>631</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>5035</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>598</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>플레이 스토어</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4961</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>선별</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>544</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>스마트 팩토리</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>995</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>행사 가격</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>596</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>트위터</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4515</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>958</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>부가가치</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>638</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>MOR</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>4305</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>454</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>4G</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>4229</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>469</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>OLED</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>4062</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>부의 효과</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>4043</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>615</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>CB</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>795</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>상품권</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>946</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>컨소시엄</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>553</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>와이파이</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>3886</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>양해각서</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>3804</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>277</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>기금</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>3715</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>1294</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>공정거래위원회</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>3578</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>